<commit_message>
massive MDY site template update
</commit_message>
<xml_diff>
--- a/raw_data/KEEN ONE/Byrnes/2014/NE Shoals Entry 2014/NE Shoals Site Info 2014.xlsx
+++ b/raw_data/KEEN ONE/Byrnes/2014/NE Shoals Entry 2014/NE Shoals Site Info 2014.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>Date Sampled</t>
   </si>
@@ -97,6 +97,15 @@
   </si>
   <si>
     <t>Broad Cove</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Year</t>
   </si>
 </sst>
 </file>
@@ -144,8 +153,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -213,7 +224,7 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="55">
+  <cellStyles count="57">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -241,6 +252,7 @@
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -268,6 +280,7 @@
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -665,21 +678,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:G2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="13.5" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="14" customHeight="1">
+    <row r="1" spans="1:17" ht="14" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -692,38 +707,47 @@
       <c r="D1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -736,38 +760,47 @@
       <c r="D2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="1">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1">
+        <v>21</v>
+      </c>
+      <c r="G2" s="1">
+        <v>2014</v>
+      </c>
+      <c r="H2" s="5">
         <v>41841</v>
       </c>
-      <c r="F2">
+      <c r="I2">
         <v>42.993069040000002</v>
       </c>
-      <c r="G2">
+      <c r="J2">
         <v>-70.613883985000001</v>
       </c>
-      <c r="H2">
+      <c r="K2">
         <v>42.99288473</v>
       </c>
-      <c r="I2">
+      <c r="L2">
         <v>-70.613730009999998</v>
       </c>
-      <c r="J2">
+      <c r="M2">
         <v>11.1</v>
       </c>
-      <c r="K2">
+      <c r="N2">
         <v>5</v>
       </c>
-      <c r="L2">
+      <c r="O2">
         <v>4</v>
       </c>
-      <c r="M2">
+      <c r="P2">
         <v>8</v>
       </c>
-      <c r="N2" t="s">
+      <c r="Q2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -780,38 +813,47 @@
       <c r="D3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="1">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1">
+        <v>2014</v>
+      </c>
+      <c r="H3" s="5">
         <v>41839</v>
       </c>
-      <c r="F3">
+      <c r="I3">
         <v>42.992762011000003</v>
       </c>
-      <c r="G3">
+      <c r="J3">
         <v>-70.611665966000004</v>
       </c>
-      <c r="H3">
+      <c r="K3">
         <v>42.993077002</v>
       </c>
-      <c r="I3">
+      <c r="L3">
         <v>-70.611877022000002</v>
       </c>
-      <c r="J3">
+      <c r="M3">
         <v>10.8</v>
       </c>
-      <c r="K3">
+      <c r="N3">
         <v>8.4</v>
       </c>
-      <c r="L3">
+      <c r="O3">
         <v>5</v>
       </c>
-      <c r="M3">
+      <c r="P3">
         <v>7</v>
       </c>
-      <c r="N3" t="s">
+      <c r="Q3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -824,38 +866,47 @@
       <c r="D4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="1">
+        <v>7</v>
+      </c>
+      <c r="F4" s="1">
+        <v>18</v>
+      </c>
+      <c r="G4" s="1">
+        <v>2014</v>
+      </c>
+      <c r="H4" s="5">
         <v>41838</v>
       </c>
-      <c r="F4">
+      <c r="I4">
         <v>42.990710958999998</v>
       </c>
-      <c r="G4">
+      <c r="J4">
         <v>-70.610730965000002</v>
       </c>
-      <c r="H4" s="2">
+      <c r="K4" s="2">
         <v>42.991084037</v>
       </c>
-      <c r="I4">
+      <c r="L4">
         <v>-70.610600039000005</v>
       </c>
-      <c r="J4">
+      <c r="M4">
         <v>9.8000000000000007</v>
       </c>
-      <c r="K4">
+      <c r="N4">
         <v>10.1</v>
       </c>
-      <c r="L4">
+      <c r="O4">
         <v>4.5</v>
       </c>
-      <c r="M4">
+      <c r="P4">
         <v>9</v>
       </c>
-      <c r="N4" t="s">
+      <c r="Q4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="1" customFormat="1">
+    <row r="5" spans="1:17" s="1" customFormat="1">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -868,65 +919,74 @@
       <c r="D5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="1">
+        <v>7</v>
+      </c>
+      <c r="F5" s="1">
+        <v>18</v>
+      </c>
+      <c r="G5" s="1">
+        <v>2014</v>
+      </c>
+      <c r="H5" s="5">
         <v>41838</v>
       </c>
-      <c r="F5">
+      <c r="I5">
         <v>42.989987014</v>
       </c>
-      <c r="G5">
+      <c r="J5">
         <v>-70.611166991000005</v>
       </c>
-      <c r="H5">
+      <c r="K5">
         <v>42.989742010999997</v>
       </c>
-      <c r="I5">
+      <c r="L5">
         <v>-70.610920981999996</v>
       </c>
-      <c r="J5">
+      <c r="M5">
         <v>6</v>
       </c>
-      <c r="K5">
+      <c r="N5">
         <v>8.4</v>
       </c>
-      <c r="L5">
+      <c r="O5">
         <v>5</v>
       </c>
-      <c r="M5">
+      <c r="P5">
         <v>9</v>
       </c>
-      <c r="N5" t="s">
+      <c r="Q5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:17">
       <c r="A6"/>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:17">
       <c r="A7"/>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:17">
       <c r="A8"/>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:17">
       <c r="A9"/>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:17">
       <c r="A10"/>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:17">
       <c r="A11"/>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:17">
       <c r="A12"/>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:17">
       <c r="A13"/>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:17">
       <c r="A14"/>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:17">
       <c r="A15"/>
     </row>
     <row r="17" spans="1:1">
@@ -953,7 +1013,7 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C74:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C74:I1048576">
       <formula1>" IN 20, IN 40, OFF 40, OFF 20"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>